<commit_message>
3rd version with the submit along with date flags
</commit_message>
<xml_diff>
--- a/form_data.xlsx
+++ b/form_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>2025-04-06 15:38:19</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:39:34</t>
         </is>
       </c>
     </row>
@@ -486,6 +491,11 @@
           <t>Submitted</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Submitted</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -509,6 +519,11 @@
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>Submitted</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Submitted</t>
         </is>

</xml_diff>

<commit_message>
4th version with the gui for the manual input of attendees
</commit_message>
<xml_diff>
--- a/form_data.xlsx
+++ b/form_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,77 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Camera On While Delivering</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Class Started on Time</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Zoom Poll Taken / Feedback Poll Taken</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total attendees (online + offline)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Resolution of Non Tech query</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Resolution of Tech query</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Refer and earn slide shown</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Participant Engagement</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Technical glitch (if any)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Was there any disruption during the session?</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Comments</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>2025-04-06 15:38:19</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>2025-04-06 15:39:34</t>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-06 18:45:35</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-06 18:46:29</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-06 18:47:54</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-06 18:49:22</t>
         </is>
       </c>
     </row>
@@ -473,25 +533,81 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>15-FEB-25-CDS-BUN-021-WEM0930-BAN &amp; 28-Dec-24-CDS-BUN-021-WEM09-BAN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>cds</t>
+          <t>29-MAR-25-MLE-113-WEM09-BAN (CONTINUE)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NA - Test</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Error: name 'tk' is not defined</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>Submitted</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Submitted</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
         <is>
           <t>Submitted</t>
         </is>
@@ -505,25 +621,83 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15-FEB-25-CDS-BUN-021-WEM0930-BAN &amp; 28-Dec-24-CDS-BUN-021-WEM09-BAN</t>
+          <t>test</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>29-MAR-25-MLE-113-WEM09-BAN (CONTINUE)</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>test wem</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>43</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>test 2</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Error: name 'tk' is not defined</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>Submitted</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Submitted</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
         <is>
           <t>Submitted</t>
         </is>

</xml_diff>

<commit_message>
5th version with email field and rating count
</commit_message>
<xml_diff>
--- a/form_data.xlsx
+++ b/form_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,268 +436,178 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>SME</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Batch Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Course Event</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Camera On While Delivering</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Class Started on Time</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Zoom Poll Taken / Feedback Poll Taken</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Total attendees (online + offline)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Resolution of Non Tech query</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Resolution of Tech query</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Refer and earn slide shown</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Participant Engagement</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Technical glitch (if any)</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Was there any disruption during the session?</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>How many ratings less than 4 for today's session? (in any category)</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Comments</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>2025-04-06 18:45:35</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>2025-04-06 18:46:29</t>
-        </is>
-      </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>2025-04-06 18:47:54</t>
+          <t>2025-05-21 10:29:35</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>2025-04-06 18:49:22</t>
+          <t>2025-05-21 10:33:14</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>shahul.s@skillfloor.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Shahul Hameed</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>15-FEB-25-CDS-BUN-021-WEM0930-BAN &amp; 28-Dec-24-CDS-BUN-021-WEM09-BAN</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>29-MAR-25-MLE-113-WEM09-BAN (CONTINUE)</t>
+          <t>17-MAR-25-CDE-BUN-031-WDE2030-ONL31-MAR-25-CDE-BUN-031-WDE2030-ONL21-APR-25-CDE-BUN-031-WDE2030-ONL</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>28-APR-25-DEA-135-WDE20-ONL (CONTINUE)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Error: name 'tk' is not defined</t>
-        </is>
+      <c r="O2" t="n">
+        <v>1</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
+          <t>Hey</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
           <t>Submitted</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
       <c r="R2" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Shahul Hameed</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>43</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>test 2</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Error: name 'tk' is not defined</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Submitted</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
         <is>
           <t>Submitted</t>
         </is>

</xml_diff>